<commit_message>
Update Updated model output 17-4-20.xlsx
</commit_message>
<xml_diff>
--- a/ms/Updated model output 17-4-20.xlsx
+++ b/ms/Updated model output 17-4-20.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurenharrison/Documents/GitHub/sex_meta/ms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2F80DB-65C0-6D4B-8146-0A0CDF266507}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50BE062B-3A94-5C43-8A32-41D41C436232}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17960" yWindow="460" windowWidth="38200" windowHeight="19700" activeTab="3" xr2:uid="{5BDBDF95-A114-D34B-9842-3CB243171EE0}"/>
+    <workbookView xWindow="160" yWindow="460" windowWidth="38200" windowHeight="19700" activeTab="3" xr2:uid="{5BDBDF95-A114-D34B-9842-3CB243171EE0}"/>
   </bookViews>
   <sheets>
     <sheet name="Intercept models" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2501" uniqueCount="545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2504" uniqueCount="547">
   <si>
     <t xml:space="preserve">Intercept only models are our most simple multilevel mixed models to compare SMD (means) and lnCVR (variance) for males and females, in each taxo group. </t>
   </si>
@@ -1663,6 +1663,12 @@
   </si>
   <si>
     <t>-6.11, 10.68</t>
+  </si>
+  <si>
+    <t>p=0.017</t>
+  </si>
+  <si>
+    <t>p=0.004</t>
   </si>
 </sst>
 </file>
@@ -2149,7 +2155,7 @@
   <dimension ref="A1:AI60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Y24" sqref="Y24"/>
+      <selection activeCell="AG37" sqref="AG37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3272,6 +3278,9 @@
       <c r="AG22" t="s">
         <v>18</v>
       </c>
+      <c r="AH22">
+        <v>11</v>
+      </c>
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
@@ -3361,6 +3370,9 @@
       <c r="AG23" s="5" t="s">
         <v>91</v>
       </c>
+      <c r="AH23" s="5">
+        <v>10</v>
+      </c>
     </row>
     <row r="24" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
@@ -3419,6 +3431,9 @@
       </c>
       <c r="AE24">
         <v>0</v>
+      </c>
+      <c r="AH24">
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:35" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -3948,7 +3963,7 @@
   <dimension ref="A1:AS39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4109,8 +4124,8 @@
       <c r="B8" s="4">
         <v>2.79</v>
       </c>
-      <c r="C8" s="4">
-        <v>1.7000000000000001E-2</v>
+      <c r="C8" s="4" t="s">
+        <v>545</v>
       </c>
       <c r="D8" t="s">
         <v>115</v>
@@ -4130,8 +4145,8 @@
       <c r="T8" s="4">
         <v>3.53</v>
       </c>
-      <c r="U8" s="4">
-        <v>4.0000000000000001E-3</v>
+      <c r="U8" s="4" t="s">
+        <v>546</v>
       </c>
       <c r="V8" s="4"/>
       <c r="AB8" s="5" t="s">
@@ -6670,7 +6685,7 @@
   <dimension ref="A1:AN79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J33" sqref="J33"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6833,8 +6848,8 @@
       <c r="J8" s="5">
         <v>0.57999999999999996</v>
       </c>
-      <c r="K8" s="5">
-        <v>0.75</v>
+      <c r="K8" s="5" t="s">
+        <v>223</v>
       </c>
       <c r="Q8" s="5" t="s">
         <v>59</v>
@@ -12144,6 +12159,7 @@
   <cols>
     <col min="1" max="1" width="15.5" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
+    <col min="11" max="11" width="12" customWidth="1"/>
     <col min="17" max="17" width="14.33203125" customWidth="1"/>
     <col min="25" max="25" width="14.83203125" customWidth="1"/>
     <col min="33" max="33" width="14.5" customWidth="1"/>

</xml_diff>